<commit_message>
bug fix in japanese NLU
</commit_message>
<xml_diff>
--- a/sample_apps/network_ja/sample-knowledge-ja.xlsx
+++ b/sample_apps/network_ja/sample-knowledge-ja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb-develop\sample_apps\network_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12369B19-6B18-439E-96FA-E79F24629EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7526313-7D15-45BC-A2A1-C076CE216C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="111">
   <si>
     <t>system utterance</t>
     <phoneticPr fontId="1"/>
@@ -761,6 +761,13 @@
     <t>(醤油)[favorite_ramen]かな</t>
     <rPh sb="1" eb="3">
       <t>ショウユ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>食べます</t>
+    <rPh sb="0" eb="1">
+      <t>タ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1184,24 +1191,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" style="4"/>
-    <col min="2" max="2" width="23.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.58203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="4"/>
+    <col min="2" max="2" width="23.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.58203125" style="4"/>
+    <col min="6" max="6" width="37.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1227,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
@@ -1244,7 +1251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1258,7 +1265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B4" s="4" t="s">
         <v>24</v>
       </c>
@@ -1272,7 +1279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1280,7 +1287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1297,7 +1304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1311,7 +1318,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1325,7 +1332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1339,7 +1346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1364,7 +1371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.4">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1387,7 +1394,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1407,7 +1414,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
@@ -1424,7 +1431,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1435,7 +1442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
@@ -1449,7 +1456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
@@ -1460,7 +1467,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B18" s="4" t="s">
         <v>33</v>
       </c>
@@ -1471,7 +1478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1482,7 +1489,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B20" s="4" t="s">
         <v>25</v>
       </c>
@@ -1490,7 +1497,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="54" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="B21" s="4" t="s">
         <v>37</v>
       </c>
@@ -1498,7 +1505,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="C29" s="4"/>
     </row>
   </sheetData>
@@ -1510,19 +1517,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8F96FF-CF47-4A99-83E7-8D5E860D6DFF}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -1533,7 +1540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1544,7 +1551,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1555,7 +1562,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1566,7 +1573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1577,7 +1584,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1588,7 +1595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1599,7 +1606,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1610,7 +1617,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1621,7 +1628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1632,7 +1639,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1643,7 +1650,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1654,7 +1661,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1665,7 +1672,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1676,7 +1683,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1687,7 +1694,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1698,7 +1705,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1709,7 +1716,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1720,7 +1727,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1731,7 +1738,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1742,7 +1749,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1753,7 +1760,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1764,7 +1771,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1775,7 +1782,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1786,7 +1793,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1797,7 +1804,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1808,7 +1815,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1819,7 +1826,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1830,7 +1837,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1841,7 +1848,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1852,7 +1859,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1863,7 +1870,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1874,7 +1881,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1885,18 +1892,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1904,10 +1911,10 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1915,10 +1922,10 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1926,10 +1933,10 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1937,10 +1944,10 @@
         <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1948,6 +1955,17 @@
         <v>33</v>
       </c>
       <c r="C39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1970,13 +1988,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="14.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1987,7 +2005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -2012,15 +2030,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2037,7 +2055,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2068,13 +2086,13 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -2088,7 +2106,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -2102,7 +2120,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2116,7 +2134,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2130,7 +2148,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -2144,7 +2162,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
issue #2 resolved, document updated
</commit_message>
<xml_diff>
--- a/sample_apps/network_ja/sample-knowledge-ja.xlsx
+++ b/sample_apps/network_ja/sample-knowledge-ja.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb-develop\sample_apps\network_ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb\sample_apps\network_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7526313-7D15-45BC-A2A1-C076CE216C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD59042-CAAE-476C-A81F-321465DE9700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="690" yWindow="1330" windowWidth="19460" windowHeight="11060" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -1191,24 +1191,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="4"/>
-    <col min="2" max="2" width="23.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" style="4"/>
+    <col min="2" max="2" width="23.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.58203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.625" style="4"/>
+    <col min="6" max="6" width="37.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.58203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="54" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="4" t="s">
         <v>24</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="54" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="54" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="4" t="s">
         <v>33</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="4" t="s">
         <v>25</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:8" ht="54" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="4" t="s">
         <v>37</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" s="4"/>
     </row>
   </sheetData>
@@ -1519,17 +1519,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8F96FF-CF47-4A99-83E7-8D5E860D6DFF}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1988,13 +1988,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -2030,15 +2030,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2086,13 +2086,13 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
doc figure updated, sample config fixed
</commit_message>
<xml_diff>
--- a/sample_apps/network_ja/sample-knowledge-ja.xlsx
+++ b/sample_apps/network_ja/sample-knowledge-ja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb\sample_apps\network_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224BA303-E5A1-4D03-BD90-3E709EDC7732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437043A2-60DD-4E26-B7B0-4A53E029E3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19400" windowHeight="11000" activeTab="4" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -1271,20 +1271,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.625" style="4"/>
-    <col min="2" max="2" width="23.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="29.625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.625" style="4" customWidth="1"/>
     <col min="9" max="16384" width="8.625" style="4"/>
   </cols>
   <sheetData>
@@ -2342,7 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60152591-03E8-42BE-B56A-8DD50B7AC6A8}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nbest nlu, column names of nlu knowledge sheets changed
</commit_message>
<xml_diff>
--- a/sample_apps/network_ja/sample-knowledge-ja.xlsx
+++ b/sample_apps/network_ja/sample-knowledge-ja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb\sample_apps\network_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437043A2-60DD-4E26-B7B0-4A53E029E3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91647112-0ECF-4B40-9FA5-3198BD2D3F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -105,10 +105,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>slot</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>はい、よく食べます。</t>
     <rPh sb="5" eb="6">
       <t>タ</t>
@@ -689,10 +685,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>synonyms</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -849,6 +841,14 @@
   </si>
   <si>
     <t>decide_greeting(&amp;greeting)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>slot name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>entity class</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1271,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1293,7 +1293,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1308,7 +1308,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
@@ -1316,30 +1316,30 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>2</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>3</v>
@@ -1367,16 +1367,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>2</v>
@@ -1384,310 +1384,310 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="H17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
@@ -1704,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8F96FF-CF47-4A99-83E7-8D5E860D6DFF}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -1727,475 +1727,475 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
@@ -2216,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E27BD90-5E4C-4A7C-B9E8-ABC211947ECB}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2231,32 +2231,32 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
         <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2270,7 +2270,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2286,24 +2286,24 @@
         <v>7</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2317,10 +2317,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -2343,11 +2343,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2357,83 +2358,83 @@
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" t="s">
-        <v>86</v>
-      </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
         <v>94</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A bug in network-ja-sample scenario fixed
</commit_message>
<xml_diff>
--- a/sample_apps/network_ja/sample-knowledge-ja.xlsx
+++ b/sample_apps/network_ja/sample-knowledge-ja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb\sample_apps\network_ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-v0.3\sample_apps\network_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91647112-0ECF-4B40-9FA5-3198BD2D3F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56B7022-415A-4A54-BBE0-1D1A4110A9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -762,10 +762,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>_set(&amp;location, #location)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>{location}ですね。今日はお時間ありがとうございました。</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -849,6 +845,10 @@
   </si>
   <si>
     <t>entity class</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_set(&amp;location, #ramen_location)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1319,10 +1319,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>22</v>
@@ -1336,7 +1336,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>14</v>
@@ -1637,10 +1637,10 @@
         <v>108</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>109</v>
@@ -1665,7 +1665,7 @@
         <v>109</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
@@ -1704,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8F96FF-CF47-4A99-83E7-8D5E860D6DFF}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -2159,10 +2159,10 @@
         <v>37</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
@@ -2170,10 +2170,10 @@
         <v>37</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
@@ -2181,10 +2181,10 @@
         <v>37</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
@@ -2192,10 +2192,10 @@
         <v>37</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
@@ -2216,7 +2216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E27BD90-5E4C-4A7C-B9E8-ABC211947ECB}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2231,10 +2231,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -2250,13 +2250,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
         <v>113</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>114</v>
-      </c>
-      <c r="C3" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2286,7 +2286,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>80</v>
@@ -2317,10 +2317,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -2358,7 +2358,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
bugs about spacy NER in docs fixed
</commit_message>
<xml_diff>
--- a/sample_apps/network_ja/sample-knowledge-ja.xlsx
+++ b/sample_apps/network_ja/sample-knowledge-ja.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-v0.3\sample_apps\network_ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb\sample_apps\network_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56B7022-415A-4A54-BBE0-1D1A4110A9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D2B45D-B13E-473B-9509-E4F3369A65AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
@@ -881,7 +881,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -912,6 +912,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -927,7 +951,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -954,6 +978,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1269,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1314,384 +1368,420 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="G2" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:8" s="11" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="G4" s="12"/>
+      <c r="H4" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="3"/>
+      <c r="H8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="G12" s="14"/>
+      <c r="H12" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.4">
-      <c r="A13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:8" s="15" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+      <c r="A13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:8" s="15" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:8" s="15" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="G16" s="16"/>
+      <c r="H16" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:8" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="G17" s="10"/>
+      <c r="H17" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:8" s="11" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="D18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="1:8" s="11" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="D19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="1:8" s="15" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A22" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="16" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="D22" s="16"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A23" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="D23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="1:8" s="11" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C32" s="4"/>
+      <c r="D24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>